<commit_message>
Tested airbnb and Chase
</commit_message>
<xml_diff>
--- a/base/src/main/resources/TestData.xlsx
+++ b/base/src/main/resources/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hafiz\IDEA Project\Team1BootCamp\base\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janna\IdeaProjects\Team1BootCamp\base\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4722EE68-90EB-42C0-AF92-D8B589C2F532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B2ED8D-B047-4ABF-AA4E-997B67673F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
+    <workbookView xWindow="5595" yWindow="855" windowWidth="21600" windowHeight="11385" activeTab="7" xr2:uid="{BF43A26A-CFA6-4A10-8339-8D5564FBA255}"/>
   </bookViews>
   <sheets>
     <sheet name="Expedia" sheetId="1" r:id="rId1"/>
@@ -28,19 +28,10 @@
     <sheet name="Mercedes-Benz" sheetId="13" r:id="rId13"/>
     <sheet name="Redfin" sheetId="14" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -403,9 +394,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F16D271-5906-41EE-853E-85EA245B6942}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -419,7 +410,7 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -433,7 +424,7 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -447,7 +438,7 @@
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -461,7 +452,7 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -475,7 +466,7 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -489,7 +480,7 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -503,7 +494,7 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -517,7 +508,7 @@
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -531,9 +522,9 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -551,7 +542,7 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -563,7 +554,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -573,11 +564,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F06E338-1C0F-45E0-B136-3FC6897D7CEC}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.85546875" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -587,7 +584,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>